<commit_message>
tried to fix the gitignore
</commit_message>
<xml_diff>
--- a/clock_counter_calcs.xlsx
+++ b/clock_counter_calcs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="977" yWindow="0" windowWidth="18540" windowHeight="10449"/>
+    <workbookView xWindow="1954" yWindow="0" windowWidth="18540" windowHeight="10449"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -398,12 +398,12 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="11.3828125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.3828125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">

</xml_diff>